<commit_message>
Cleanup in ods and xlsx as per cleanup in template
</commit_message>
<xml_diff>
--- a/FindSim-Exptworksheet.xlsx
+++ b/FindSim-Exptworksheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="978" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="FindSim_worksheet" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="FindSim-worksheet" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -135,11 +135,25 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
+          <t xml:space="preserve">exptType is the broad category of the experiment.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
           <t xml:space="preserve">Species in which the experiment was done</t>
         </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="0">
+    <comment ref="A13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -153,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A15" authorId="0">
+    <comment ref="A16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -167,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A16" authorId="0">
+    <comment ref="A17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -181,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A18" authorId="0">
+    <comment ref="A19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -197,7 +211,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="0">
+    <comment ref="A20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -211,7 +225,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0">
+    <comment ref="A21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -225,7 +239,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A21" authorId="0">
+    <comment ref="A22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -239,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A22" authorId="0">
+    <comment ref="A23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -253,7 +267,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="0">
+    <comment ref="A24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -264,7 +278,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">This specifies the start line of the data block of each stimulus.
-time-value pair.</t>
+time-value pair or Entity-value pair.</t>
         </r>
       </text>
     </comment>
@@ -292,7 +306,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Readout type is the broad category of readout. </t>
+          <t xml:space="preserve">Units of time for data. Typically seconds.</t>
         </r>
       </text>
     </comment>
@@ -306,7 +320,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Units of time for data. Typically seconds.</t>
+          <t xml:space="preserve">Units of quantity for data. Typically uM, that is micromolar</t>
         </r>
       </text>
     </comment>
@@ -320,7 +334,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Units of quantity for data. Typically uM, that is micromolar</t>
+          <t xml:space="preserve">Use logarithmic scaling for X axis.</t>
         </r>
       </text>
     </comment>
@@ -334,7 +348,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Use logarithmic scaling for X axis.</t>
+          <t xml:space="preserve">Use logarithmic scaling for Y axis</t>
         </r>
       </text>
     </comment>
@@ -348,25 +362,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Use logarithmic scaling for Y axis</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A33" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
           <t xml:space="preserve">Normalizating the value to the first "Data" point</t>
         </r>
       </text>
     </comment>
-    <comment ref="A35" authorId="0">
+    <comment ref="A34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -382,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A36" authorId="0">
+    <comment ref="A35" authorId="0">
       <text>
         <r>
           <rPr>
@@ -397,7 +397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A38" authorId="0">
+    <comment ref="A37" authorId="0">
       <text>
         <r>
           <rPr>
@@ -412,6 +412,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="A38" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Field to monitor in the readout. </t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A39" authorId="0">
       <text>
         <r>
@@ -422,24 +436,24 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Field to monitor in the readout. </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A40" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
           <t xml:space="preserve">Data block for experimental data, corresponding to block above. 3 columns. Can repeat.</t>
         </r>
       </text>
     </comment>
+    <comment ref="A43" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">The block specifies the model source used to run simulation</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A44" authorId="0">
       <text>
         <r>
@@ -450,7 +464,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">The block specifies the model source used to run simulation</t>
+          <t xml:space="preserve">This is the type of source for the model, such as a paper or database</t>
         </r>
       </text>
     </comment>
@@ -464,7 +478,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">This is the type of source for the model, such as a paper or database</t>
+          <t xml:space="preserve">Path to the model file for loading</t>
         </r>
       </text>
     </comment>
@@ -478,7 +492,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Path to the model file for loading</t>
+          <t xml:space="preserve">The URL or accession number of the model in a database.</t>
         </r>
       </text>
     </comment>
@@ -492,7 +506,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">The URL or accession number of the model in a database.</t>
+          <t xml:space="preserve">DOI for the paper</t>
         </r>
       </text>
     </comment>
@@ -506,7 +520,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">DOI for the paper</t>
+          <t xml:space="preserve">Author list, one author per column.</t>
         </r>
       </text>
     </comment>
@@ -520,7 +534,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Author list, one author per column.</t>
+          <t xml:space="preserve">Default is all, groups with in the model that is to be retained. In one cell, in the MOOSE format, with commas as separators between further subsets</t>
         </r>
       </text>
     </comment>
@@ -534,24 +548,24 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Default is all, groups with in the model that is to be retained. In one cell, in the MOOSE format, with commas as separators between further subsets</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A51" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
           <t xml:space="preserve">This would be species map from the `Stimulus-&gt;molecule` block's to species map to the model</t>
         </r>
       </text>
     </comment>
+    <comment ref="A53" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Which numerical method to use for the simulation.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A54" authorId="0">
       <text>
         <r>
@@ -562,7 +576,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Which numerical method to use for the simulation.</t>
+          <t xml:space="preserve">Curator notes</t>
         </r>
       </text>
     </comment>
@@ -576,25 +590,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Curator notes</t>
+          <t xml:space="preserve">Parameters to change from the original model. One can change any number of such parameters, and each one is on a new line. For example, the baseline concentration of one molecule may be changed for the purposes of an experiment, to represent the presence of a blocker in that experiment. Additionally the forward rate constant of a reaction may change. Each line here has four colums: 1. The parameterChange keyword. 2. The full MOOSE path of the object which is being changed. 3. The field of this object to change and 4. The new value of the object.</t>
         </r>
       </text>
     </comment>
     <comment ref="A56" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Parameters to change from the original model. One can change any number of such parameters, and each one is on a new line. For example, the baseline concentration of one molecule may be changed for the purposes of an experiment, to represent the presence of a blocker in that experiment. Additionally the forward rate constant of a reaction may change. Each line here has four colums: 1. The parameterChange keyword. 2. The full MOOSE path of the object which is being changed. 3. The field of this object to change and 4. The new value of the object.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A57" authorId="0">
       <text>
         <r>
           <rPr>
@@ -613,7 +613,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
   <si>
     <t xml:space="preserve">Experiment metadata</t>
   </si>
@@ -648,6 +648,12 @@
     <t xml:space="preserve">Experiment context</t>
   </si>
   <si>
+    <t xml:space="preserve">exptType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TimeSeries</t>
+  </si>
+  <si>
     <t xml:space="preserve">species</t>
   </si>
   <si>
@@ -687,6 +693,9 @@
     <t xml:space="preserve">field</t>
   </si>
   <si>
+    <t xml:space="preserve">concInit</t>
+  </si>
+  <si>
     <t xml:space="preserve">Data</t>
   </si>
   <si>
@@ -699,12 +708,6 @@
     <t xml:space="preserve">Readouts</t>
   </si>
   <si>
-    <t xml:space="preserve">readoutType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TimeSeries</t>
-  </si>
-  <si>
     <t xml:space="preserve">mV</t>
   </si>
   <si>
@@ -781,9 +784,6 @@
   </si>
   <si>
     <t xml:space="preserve">parameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">concInit</t>
   </si>
 </sst>
 </file>
@@ -819,22 +819,23 @@
     <font>
       <b val="true"/>
       <sz val="14"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF434343"/>
       <name val="Courier New"/>
       <family val="3"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
+      <color rgb="FF434343"/>
+      <name val="Courier new"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF999999"/>
-      <name val="Cambria"/>
-      <family val="1"/>
+      <name val="Courier new"/>
+      <family val="3"/>
       <charset val="1"/>
     </font>
     <font>
@@ -845,22 +846,20 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF434343"/>
       <name val="Courier New"/>
       <family val="3"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <color rgb="FF434343"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Courier New"/>
+      <sz val="12"/>
+      <name val="Courier new"/>
       <family val="3"/>
       <charset val="1"/>
     </font>
@@ -871,14 +870,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF434343"/>
-      <name val="Cambria"/>
-      <family val="1"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Courier new"/>
+      <family val="3"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -887,8 +886,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFF3F3F3"/>
       </patternFill>
     </fill>
   </fills>
@@ -902,16 +907,16 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="hair">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFEEEEEE"/>
       </left>
       <right style="hair">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFEEEEEE"/>
       </right>
       <top style="hair">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFEEEEEE"/>
       </top>
       <bottom style="hair">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFEEEEEE"/>
       </bottom>
       <diagonal/>
     </border>
@@ -941,68 +946,76 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1040,12 +1053,12 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFF3F3F3"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -1092,91 +1105,92 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.5357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="14.1734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
@@ -1185,496 +1199,499 @@
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="8"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="8"/>
+      <c r="C17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="9" t="s">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="6"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9" t="s">
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="s">
+      <c r="C20" s="9"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
+      <c r="B21" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="6"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9" t="s">
+      <c r="B22" s="6"/>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B23" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="8"/>
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="9"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="s">
+      <c r="A27" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="9"/>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="s">
+      <c r="B28" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="9" t="n">
+      <c r="C29" s="6"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="12"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C31" s="11"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="9" t="n">
+      <c r="C30" s="13"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C32" s="9"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="9" t="n">
-        <f aca="false">IF(B28="TimeSeries-RatioNormalization",1,0)</f>
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C33" s="12"/>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="9" t="n">
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="C34" s="9"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="9" t="n">
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="6" t="n">
         <v>-1</v>
       </c>
-      <c r="C35" s="9"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="9" t="s">
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" s="9" t="s">
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="9"/>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="9" t="s">
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="12"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="14"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B41" s="9" t="s">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="15"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+    </row>
+    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="6"/>
+      <c r="D44" s="17"/>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="14"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="17"/>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="17"/>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="14"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="17"/>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="17"/>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="6"/>
+      <c r="D49" s="17"/>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="17"/>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="17"/>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="17"/>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53" s="6"/>
+      <c r="D53" s="17"/>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="17"/>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="17"/>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D56" s="17"/>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="6"/>
+      <c r="B57" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-    </row>
-    <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C45" s="9"/>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B46" s="12"/>
-      <c r="C46" s="9"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B48" s="12"/>
-      <c r="C48" s="9"/>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C50" s="9"/>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C52" s="9"/>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C54" s="9"/>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="9"/>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="9"/>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C57" s="14"/>
+      <c r="D57" s="17"/>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6"/>
       <c r="B58" s="6" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C58" s="14"/>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D58" s="17"/>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="6"/>
       <c r="B59" s="6" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C59" s="14"/>
+      <c r="D59" s="17"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="6"/>
-      <c r="B60" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C60" s="14"/>
-    </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="15"/>
-      <c r="B61" s="15"/>
-      <c r="C61" s="15"/>
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
     <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A43:C43"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3">
+  <conditionalFormatting sqref="B2:B4,B6:B8,B12:B17">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>optional</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(TRIM(B3))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(TRIM(B3))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(TRIM(B20))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="16">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B28" type="list">
-      <formula1>"TimeSeries,DoseResponse"</formula1>
+  <dataValidations count="14">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="A40" type="list">
+      <formula1>"Time,Dose,Entity"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B5" type="list">
       <formula1>"Paper,InHouse,experiment"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="A41" type="list">
-      <formula1>"Time,Dose"</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B20 B28" type="list">
+      <formula1>"sec,millisec,microsec,nanosec,min,hrs,days"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B45" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B44" type="list">
       <formula1>"Local path,DOQCS,BioModels"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="if readoutType=&quot;TimeSeries-RatioNormalization&quot; ,useNormalization=True, rest False" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B33" type="list">
-      <formula1>"TRUE,FALSE"</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B21 B29" type="list">
+      <formula1>"M,mM,uM,nM,pM,mV,uV,V,mA,uA,nA,pA,number,ratio"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="False or True" showDropDown="true" showErrorMessage="true" showInputMessage="true" sqref="C31" type="custom">
-      <formula1>IF(B28="TimeSeries",0,1)</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B22" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B23" type="list">
       <formula1>"nInit,n,conc,concInit,inject,Vclamp"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B30" type="list">
-      <formula1>"A,mA,uA,nA,V,mV,uV,nV,ratio"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B58:B60" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B57:B59" type="list">
       <formula1>"concInit,nInit,Kf,Kb,Km,kcat,isBuffered"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Click and enter a value from the list of items" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B31:B32" type="list">
+    <dataValidation allowBlank="true" operator="between" prompt="Click and enter a value from the list of items" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B30:B32" type="list">
       <formula1>"FALSE,TRUE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B39" type="list">
+    <dataValidation allowBlank="true" operator="between" prompt="for &quot;TimeSeries-WithinstantaneousRatio&quot;,value has to be -1" showDropDown="true" showErrorMessage="true" showInputMessage="true" sqref="B33" type="custom">
+      <formula1>IF(B27="TimeSeries-WithinstantaneousRatio",-1,B33=B33)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B38" type="list">
       <formula1>"conc,n,Vm"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="for &quot;TimeSeries-WithinstantaneousRatio&quot;,value has to be -1" showDropDown="true" showErrorMessage="true" showInputMessage="true" sqref="B34:B35" type="custom">
-      <formula1>IF(B27="TimeSeries-WithinstantaneousRatio",-1,B34=B34)</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="A25" type="list">
+      <formula1>"Time,Entity"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Click and enter a value from the list of itemsmM,uM,nM,M,mV,uV,V,mA,uA,nA,pA,number,ratio" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="E2" type="list">
-      <formula1>"mM,uM,nM,M,mV,uV,V,mA,uA,nA,pA,number,ratio"</formula1>
+    <dataValidation allowBlank="true" operator="between" prompt="False or True" showDropDown="true" showErrorMessage="true" showInputMessage="true" sqref="C30" type="custom">
+      <formula1>IF(#ref!="TimeSeries",0,1)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B19 B29" type="list">
-      <formula1>"sec,millisec,nanosec"</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B11" type="list">
+      <formula1>"TimeSeries,DoseResponse,BarChart"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B20" type="list">
-      <formula1>"mM,uM,nM,M,mV,uV,V,mA,uA,nA,pA,number,ratio"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B54" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B53" type="list">
       <formula1>"Runge kutta method (gsl),stochastic simulation (gssa),exponential euler method (ee)"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>